<commit_message>
Oskuste filter, mis ei tööta
</commit_message>
<xml_diff>
--- a/Ylesanded.xlsx
+++ b/Ylesanded.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055"/>
   </bookViews>
   <sheets>
     <sheet name="Leht1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="24">
   <si>
     <t>Funktsionaalsused: </t>
   </si>
@@ -433,191 +433,258 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C23"/>
+  <dimension ref="B2:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="50.5703125" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="3">
         <v>42766</v>
       </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="3">
+        <v>42776</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="2:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="5" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="6" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C6" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="7" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C7" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="8" spans="2:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C8" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C9" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="10" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C10" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="11" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C11" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="12" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C12" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C13" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="14" spans="2:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C14" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="15" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C15" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="16" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C16" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C17" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="18" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C18" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="19" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C19" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="20" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C20" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="21" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C21" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="22" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C22" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="23" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
         <v>21</v>
       </c>
       <c r="C23" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Töötaja muudatused KL peale
</commit_message>
<xml_diff>
--- a/Ylesanded.xlsx
+++ b/Ylesanded.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17766"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PaarisProged\TootajaOskused\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GITist\PaarisProged\tootajaoskused\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -436,7 +436,7 @@
   <dimension ref="B2:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -542,7 +542,7 @@
         <v>23</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="30" x14ac:dyDescent="0.25">

</xml_diff>